<commit_message>
implantei o setOnItemClickListinner nas imagens, preciso só organizar as fotos de acordo com o segmento a que pertencem.
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -363,12 +363,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -484,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -515,7 +521,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,7 +542,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,13 +876,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -867,13 +892,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -909,7 +934,7 @@
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -988,7 +1013,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="21" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1010,7 +1035,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="21" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1021,7 +1046,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="21" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1035,20 +1060,20 @@
       <c r="E16" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1077,7 +1102,7 @@
       <c r="C22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1168,27 +1193,29 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="26" customWidth="1"/>
+    <col min="3" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1198,7 +1225,7 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1218,7 +1245,7 @@
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1238,10 +1265,10 @@
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="21" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1258,7 +1285,7 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1267,7 +1294,7 @@
       <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="21" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1278,7 +1305,7 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1287,7 +1314,7 @@
       <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="4"/>
@@ -1296,7 +1323,7 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="20" t="s">
         <v>74</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1305,7 +1332,7 @@
       <c r="D8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="21" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="4"/>
@@ -1314,7 +1341,7 @@
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="21" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1323,7 +1350,7 @@
       <c r="D9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="21" t="s">
         <v>86</v>
       </c>
       <c r="F9" s="4"/>
@@ -1332,7 +1359,7 @@
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1350,7 +1377,7 @@
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="20" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="4"/>
@@ -1364,7 +1391,7 @@
       <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="4"/>
@@ -1378,7 +1405,7 @@
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="20" t="s">
         <v>84</v>
       </c>
       <c r="C13" s="4"/>
@@ -1392,7 +1419,7 @@
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="21" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="4"/>
@@ -1406,7 +1433,7 @@
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C15" s="4"/>
@@ -1420,7 +1447,7 @@
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="21" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1"/>
@@ -1434,7 +1461,7 @@
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="1"/>
@@ -1448,7 +1475,7 @@
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="20" t="s">
         <v>81</v>
       </c>
       <c r="C18" s="1"/>
@@ -1462,11 +1489,11 @@
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="20" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="21" t="s">
         <v>59</v>
       </c>
       <c r="E19" s="1"/>
@@ -1476,11 +1503,11 @@
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="20" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="21" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="1"/>
@@ -1490,7 +1517,7 @@
       <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="20" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="1"/>
@@ -1502,7 +1529,7 @@
       <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="20" t="s">
         <v>77</v>
       </c>
       <c r="C22" s="1"/>
@@ -1512,7 +1539,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="1"/>
@@ -1522,7 +1549,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="22" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="8"/>
@@ -1547,7 +1574,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,12 +1583,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1618,7 +1645,7 @@
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1632,7 +1659,7 @@
       <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="4"/>
@@ -1644,7 +1671,7 @@
       <c r="B8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="21" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="4"/>
@@ -1656,7 +1683,7 @@
       <c r="B9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D9" s="4"/>
@@ -1757,7 +1784,7 @@
       <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="21" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="1"/>
@@ -1767,7 +1794,7 @@
       <c r="A20" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="27" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="8"/>

</xml_diff>

<commit_message>
bloquiei o print screen e a rotação de tela.
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Supermercado" sheetId="1" r:id="rId1"/>
@@ -521,27 +521,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -562,6 +541,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -876,13 +876,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -892,13 +892,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -934,7 +934,7 @@
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -1013,7 +1013,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="14" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1060,20 +1060,20 @@
       <c r="E16" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1102,7 +1102,7 @@
       <c r="C22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1192,30 +1192,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="19" customWidth="1"/>
     <col min="3" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="23"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1225,7 +1225,7 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1245,10 +1245,10 @@
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1265,10 +1265,10 @@
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="14" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1285,7 +1285,7 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1294,7 +1294,7 @@
       <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="14" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1305,7 +1305,7 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1314,7 +1314,7 @@
       <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="4"/>
@@ -1323,7 +1323,7 @@
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1332,7 +1332,7 @@
       <c r="D8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="4"/>
@@ -1341,7 +1341,7 @@
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="14" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1350,7 +1350,7 @@
       <c r="D9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="14" t="s">
         <v>86</v>
       </c>
       <c r="F9" s="4"/>
@@ -1359,10 +1359,10 @@
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1377,7 +1377,7 @@
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="4"/>
@@ -1391,7 +1391,7 @@
       <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="4"/>
@@ -1405,7 +1405,7 @@
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C13" s="4"/>
@@ -1419,7 +1419,7 @@
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C14" s="4"/>
@@ -1433,7 +1433,7 @@
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C15" s="4"/>
@@ -1447,7 +1447,7 @@
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1"/>
@@ -1461,7 +1461,7 @@
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="1"/>
@@ -1475,7 +1475,7 @@
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C18" s="1"/>
@@ -1489,11 +1489,11 @@
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="14" t="s">
         <v>59</v>
       </c>
       <c r="E19" s="1"/>
@@ -1503,11 +1503,11 @@
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="14" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="1"/>
@@ -1517,7 +1517,7 @@
       <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="1"/>
@@ -1529,7 +1529,7 @@
       <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="13" t="s">
         <v>77</v>
       </c>
       <c r="C22" s="1"/>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="1"/>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="8"/>
@@ -1583,12 +1583,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1645,7 +1645,7 @@
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1659,7 +1659,7 @@
       <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="4"/>
@@ -1671,7 +1671,7 @@
       <c r="B8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="4"/>
@@ -1683,7 +1683,7 @@
       <c r="B9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D9" s="4"/>
@@ -1784,7 +1784,7 @@
       <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="1"/>
@@ -1794,7 +1794,7 @@
       <c r="A20" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="20" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="8"/>

</xml_diff>

<commit_message>
incluí novas fotos e tirei os planos de fundo para começar a modelar o visual do aplicativo.
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Supermercado" sheetId="1" r:id="rId1"/>
     <sheet name="Restaurante" sheetId="4" r:id="rId2"/>
     <sheet name="Hotelaria" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +937,7 @@
       <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -985,7 +985,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4"/>
@@ -1024,7 +1024,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="14" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       <c r="B22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="12" t="s">
@@ -1120,7 +1120,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,10 +1254,10 @@
       <c r="D4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="14" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -1356,7 +1356,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -1368,7 +1368,7 @@
       <c r="D10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="14" t="s">
         <v>87</v>
       </c>
       <c r="F10" s="4"/>
@@ -1409,7 +1409,7 @@
         <v>84</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="4"/>
@@ -1479,7 +1479,7 @@
         <v>81</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="14" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="1"/>
@@ -1573,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,10 +1617,10 @@
       <c r="B4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1634,7 +1634,7 @@
       <c r="C5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1689,13 +1689,13 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="14" t="s">
         <v>87</v>
       </c>
       <c r="D10" s="4"/>
@@ -1774,7 +1774,7 @@
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
fiz a divisão entre consumo e revenda do segmento de supermercados e adicionei novas imagens.
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Supermercado" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="109">
   <si>
     <t>Descartáveis</t>
   </si>
@@ -340,13 +340,16 @@
   </si>
   <si>
     <t>AUDAX</t>
+  </si>
+  <si>
+    <t>(não temos)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,8 +365,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -540,6 +562,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -866,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,13 +904,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -892,13 +920,13 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -931,7 +959,7 @@
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -948,10 +976,10 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -965,9 +993,11 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -980,7 +1010,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -991,7 +1021,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1002,7 +1032,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="21" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1060,20 +1090,20 @@
       <c r="E16" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1193,7 +1223,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,14 +1234,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1288,7 +1318,7 @@
       <c r="B6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1308,7 +1338,7 @@
       <c r="B7" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="14" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1326,7 +1356,7 @@
       <c r="B8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1344,7 +1374,7 @@
       <c r="B9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="14" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1573,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,12 +1613,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>

</xml_diff>

<commit_message>
adicionei os produtos da galvanotek, falta segmentar os produtos.
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
alterei as planilhas e o txt do banco
</commit_message>
<xml_diff>
--- a/CATÁLOGOS.xlsx
+++ b/CATÁLOGOS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="8010"/>
@@ -10,6 +10,7 @@
     <sheet name="Supermercado" sheetId="1" r:id="rId1"/>
     <sheet name="Restaurante" sheetId="4" r:id="rId2"/>
     <sheet name="Hotelaria" sheetId="5" r:id="rId3"/>
+    <sheet name="Plan1" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -894,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1223,7 +1224,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1433,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -1446,7 +1447,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="14" t="s">
@@ -1460,7 +1461,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -1604,7 +1605,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1732,7 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1741,7 +1742,7 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1751,7 +1752,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1837,4 +1838,16 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>